<commit_message>
Excel File generated, Waiting for validation
</commit_message>
<xml_diff>
--- a/Termes-interdits-poclain-CN-YUAN-V2.xlsx
+++ b/Termes-interdits-poclain-CN-YUAN-V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PoclainVerification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE828044-8982-41A5-9D7B-CD855F8E0601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D07CC6-BB95-428C-8D3A-ED2B4A98BE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="417">
   <si>
     <t>Adresse</t>
   </si>
@@ -992,9 +992,6 @@
     <t>58: 世界级</t>
   </si>
   <si>
-    <t>59: 顶级（顶尖/尖端）</t>
-  </si>
-  <si>
     <t>60: 顶级工艺</t>
   </si>
   <si>
@@ -1005,9 +1002,6 @@
   </si>
   <si>
     <t>63: 极品</t>
-  </si>
-  <si>
-    <t>64: 极佳（绝佳/绝对）</t>
   </si>
   <si>
     <t>65: 终极</t>
@@ -1061,9 +1055,6 @@
     <t>81: 填补国内空白</t>
   </si>
   <si>
-    <t>82: 中国驰名（驰名商标）</t>
-  </si>
-  <si>
     <t>83: 国际品质</t>
   </si>
   <si>
@@ -1086,9 +1077,6 @@
   </si>
   <si>
     <t>7: 世界领先</t>
-  </si>
-  <si>
-    <t>8: （遥遥）领先</t>
   </si>
   <si>
     <t>9: 领导者</t>
@@ -1269,6 +1257,46 @@
   </si>
   <si>
     <t>68: 卖/抢疯了</t>
+  </si>
+  <si>
+    <t>69: 绝佳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>70: 绝对</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>64: 极佳</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>71: 顶尖</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>72: 尖端</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>59: 顶级</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>73: 驰名商标</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>82: 中国驰名</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>8: （遥遥）领先</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>74: 遥遥领先</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1662,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FB125"/>
+  <dimension ref="A1:FH125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DT1" workbookViewId="0">
-      <selection activeCell="FC1" sqref="FC1"/>
+    <sheetView tabSelected="1" topLeftCell="EC1" workbookViewId="0">
+      <selection activeCell="EN24" sqref="EN24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1676,7 +1704,7 @@
     <col min="123" max="123" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1873,286 +1901,304 @@
         <v>317</v>
       </c>
       <c r="BN1" t="s">
+        <v>412</v>
+      </c>
+      <c r="BO1" t="s">
         <v>318</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>319</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>320</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>321</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BT1" t="s">
         <v>322</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>323</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>324</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
         <v>325</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>326</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>327</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BZ1" t="s">
         <v>328</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CA1" t="s">
         <v>329</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CB1" t="s">
         <v>330</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
         <v>331</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CD1" t="s">
         <v>332</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CE1" t="s">
         <v>333</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CF1" t="s">
         <v>334</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CG1" t="s">
         <v>335</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CH1" t="s">
         <v>336</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CI1" t="s">
         <v>337</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CJ1" t="s">
         <v>338</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CK1" t="s">
+        <v>414</v>
+      </c>
+      <c r="CL1" t="s">
         <v>339</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CM1" t="s">
         <v>340</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CN1" t="s">
         <v>341</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CO1" t="s">
         <v>342</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CP1" t="s">
         <v>343</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CQ1" t="s">
         <v>344</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CR1" t="s">
         <v>345</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CS1" t="s">
         <v>346</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CT1" t="s">
+        <v>415</v>
+      </c>
+      <c r="CU1" t="s">
         <v>347</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CV1" t="s">
         <v>348</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CW1" t="s">
         <v>349</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CX1" t="s">
         <v>350</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CY1" t="s">
         <v>351</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CZ1" t="s">
         <v>352</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DA1" t="s">
         <v>353</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DB1" t="s">
         <v>354</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DC1" t="s">
         <v>355</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DD1" t="s">
         <v>356</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DE1" t="s">
         <v>357</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DF1" t="s">
         <v>358</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DG1" t="s">
         <v>359</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DH1" t="s">
         <v>360</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DI1" t="s">
         <v>361</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DJ1" t="s">
         <v>362</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DK1" t="s">
         <v>363</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DL1" t="s">
         <v>364</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DM1" t="s">
         <v>365</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DN1" t="s">
         <v>366</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DO1" t="s">
         <v>367</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DP1" t="s">
         <v>368</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DQ1" t="s">
         <v>369</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DR1" t="s">
         <v>370</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DS1" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DT1" t="s">
         <v>372</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DU1" t="s">
         <v>373</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DV1" t="s">
         <v>374</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DW1" t="s">
         <v>375</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DX1" t="s">
         <v>376</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DY1" t="s">
         <v>377</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DZ1" t="s">
         <v>378</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="EA1" t="s">
         <v>379</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="EB1" t="s">
         <v>380</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="EC1" t="s">
         <v>381</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="ED1" t="s">
         <v>382</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EE1" t="s">
         <v>383</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EF1" t="s">
         <v>384</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="EG1" t="s">
         <v>385</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EH1" t="s">
         <v>386</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EI1" t="s">
         <v>387</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EJ1" t="s">
         <v>388</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EK1" t="s">
         <v>389</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EL1" t="s">
         <v>390</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EM1" t="s">
         <v>391</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EN1" t="s">
         <v>392</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EO1" t="s">
         <v>393</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EP1" t="s">
         <v>394</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EQ1" t="s">
         <v>395</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="ER1" t="s">
         <v>396</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="ES1" t="s">
         <v>397</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="ET1" t="s">
         <v>398</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="EU1" t="s">
         <v>399</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="EV1" t="s">
         <v>400</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="EW1" t="s">
         <v>401</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EX1" t="s">
         <v>402</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EY1" t="s">
         <v>403</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EZ1" t="s">
         <v>404</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="FA1" t="s">
         <v>405</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="FB1" t="s">
         <v>406</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FC1" t="s">
         <v>407</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FD1" t="s">
         <v>408</v>
       </c>
-      <c r="FA1" t="s">
-        <v>409</v>
-      </c>
-      <c r="FB1" t="s">
+      <c r="FE1" t="s">
         <v>410</v>
       </c>
+      <c r="FF1" t="s">
+        <v>411</v>
+      </c>
+      <c r="FG1" t="s">
+        <v>413</v>
+      </c>
+      <c r="FH1" t="s">
+        <v>416</v>
+      </c>
     </row>
-    <row r="2" spans="1:158" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -2621,8 +2667,26 @@
       <c r="FB2">
         <v>0</v>
       </c>
+      <c r="FC2">
+        <v>0</v>
+      </c>
+      <c r="FD2">
+        <v>0</v>
+      </c>
+      <c r="FE2">
+        <v>0</v>
+      </c>
+      <c r="FF2">
+        <v>0</v>
+      </c>
+      <c r="FG2">
+        <v>0</v>
+      </c>
+      <c r="FH2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3094,8 +3158,26 @@
       <c r="FB3" s="2">
         <v>0</v>
       </c>
+      <c r="FC3" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD3" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE3" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF3" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG3" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -3567,8 +3649,26 @@
       <c r="FB4" s="2">
         <v>0</v>
       </c>
+      <c r="FC4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -4040,8 +4140,26 @@
       <c r="FB5" s="2">
         <v>0</v>
       </c>
+      <c r="FC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE5" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF5" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG5" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>83</v>
       </c>
@@ -4513,8 +4631,26 @@
       <c r="FB6" s="2">
         <v>0</v>
       </c>
+      <c r="FC6" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE6" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG6" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH6" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>89</v>
       </c>
@@ -4986,8 +5122,26 @@
       <c r="FB7" s="2">
         <v>0</v>
       </c>
+      <c r="FC7" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD7" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE7" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG7" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH7" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -5459,8 +5613,26 @@
       <c r="FB8" s="1">
         <v>0</v>
       </c>
+      <c r="FC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
@@ -5932,8 +6104,26 @@
       <c r="FB9" s="1">
         <v>0</v>
       </c>
+      <c r="FC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -6405,8 +6595,26 @@
       <c r="FB10" s="1">
         <v>0</v>
       </c>
+      <c r="FC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
@@ -6878,8 +7086,26 @@
       <c r="FB11" s="1">
         <v>0</v>
       </c>
+      <c r="FC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE11" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG11" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -7351,8 +7577,26 @@
       <c r="FB12" s="1">
         <v>0</v>
       </c>
+      <c r="FC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE12" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG12" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -7824,8 +8068,26 @@
       <c r="FB13" s="1">
         <v>0</v>
       </c>
+      <c r="FC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD13" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE13" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG13" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -8297,8 +8559,26 @@
       <c r="FB14" s="1">
         <v>0</v>
       </c>
+      <c r="FC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD14" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE14" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF14" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG14" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
@@ -8770,8 +9050,26 @@
       <c r="FB15" s="1">
         <v>0</v>
       </c>
+      <c r="FC15" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD15" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE15" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF15" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG15" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH15" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -9243,8 +9541,26 @@
       <c r="FB16" s="1">
         <v>0</v>
       </c>
+      <c r="FC16" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD16" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE16" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF16" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG16" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH16" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -9716,8 +10032,26 @@
       <c r="FB17" s="1">
         <v>0</v>
       </c>
+      <c r="FC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH17" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -10189,8 +10523,26 @@
       <c r="FB18" s="1">
         <v>0</v>
       </c>
+      <c r="FC18" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE18" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF18" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG18" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH18" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -10662,8 +11014,26 @@
       <c r="FB19" s="1">
         <v>0</v>
       </c>
+      <c r="FC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE19" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF19" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG19" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH19" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -11135,8 +11505,26 @@
       <c r="FB20" s="1">
         <v>0</v>
       </c>
+      <c r="FC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE20" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG20" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH20" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:158" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:164" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>91</v>
       </c>
@@ -11608,8 +11996,26 @@
       <c r="FB21" s="2">
         <v>0</v>
       </c>
+      <c r="FC21" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD21" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE21" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF21" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG21" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH21" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -12081,8 +12487,26 @@
       <c r="FB22" s="1">
         <v>0</v>
       </c>
+      <c r="FC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE22" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG22" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH22" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -12554,8 +12978,26 @@
       <c r="FB23" s="1">
         <v>0</v>
       </c>
+      <c r="FC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE23" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF23" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG23" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH23" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -13027,8 +13469,26 @@
       <c r="FB24" s="1">
         <v>0</v>
       </c>
+      <c r="FC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE24" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF24" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG24" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH24" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -13500,8 +13960,26 @@
       <c r="FB25" s="1">
         <v>0</v>
       </c>
+      <c r="FC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF25" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG25" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH25" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -13973,8 +14451,26 @@
       <c r="FB26" s="1">
         <v>0</v>
       </c>
+      <c r="FC26" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE26" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF26" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG26" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH26" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>157</v>
       </c>
@@ -14446,8 +14942,26 @@
       <c r="FB27" s="1">
         <v>0</v>
       </c>
+      <c r="FC27" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD27" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE27" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF27" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG27" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH27" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>131</v>
       </c>
@@ -14919,8 +15433,26 @@
       <c r="FB28" s="1">
         <v>0</v>
       </c>
+      <c r="FC28" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD28" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE28" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF28" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG28" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH28" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>129</v>
       </c>
@@ -15392,8 +15924,26 @@
       <c r="FB29" s="1">
         <v>0</v>
       </c>
+      <c r="FC29" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD29" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE29" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF29" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG29" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH29" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -15865,8 +16415,26 @@
       <c r="FB30" s="1">
         <v>0</v>
       </c>
+      <c r="FC30" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD30" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE30" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF30" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG30" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH30" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>177</v>
       </c>
@@ -16338,8 +16906,26 @@
       <c r="FB31" s="1">
         <v>0</v>
       </c>
+      <c r="FC31" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD31" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE31" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF31" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG31" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH31" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>221</v>
       </c>
@@ -16811,8 +17397,26 @@
       <c r="FB32" s="1">
         <v>0</v>
       </c>
+      <c r="FC32" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD32" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE32" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF32" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG32" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH32" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>207</v>
       </c>
@@ -17284,8 +17888,26 @@
       <c r="FB33" s="1">
         <v>0</v>
       </c>
+      <c r="FC33" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD33" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE33" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF33" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG33" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH33" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>153</v>
       </c>
@@ -17757,8 +18379,26 @@
       <c r="FB34" s="1">
         <v>0</v>
       </c>
+      <c r="FC34" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD34" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE34" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG34" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH34" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>159</v>
       </c>
@@ -18230,8 +18870,26 @@
       <c r="FB35" s="1">
         <v>0</v>
       </c>
+      <c r="FC35" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD35" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE35" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF35" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG35" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH35" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>217</v>
       </c>
@@ -18703,8 +19361,26 @@
       <c r="FB36" s="1">
         <v>0</v>
       </c>
+      <c r="FC36" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD36" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE36" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF36" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG36" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH36" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -19176,8 +19852,26 @@
       <c r="FB37" s="1">
         <v>0</v>
       </c>
+      <c r="FC37" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD37" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE37" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF37" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG37" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH37" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>258</v>
       </c>
@@ -19649,8 +20343,26 @@
       <c r="FB38" s="1">
         <v>0</v>
       </c>
+      <c r="FC38" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD38" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE38" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF38" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG38" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH38" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>189</v>
       </c>
@@ -20122,8 +20834,26 @@
       <c r="FB39" s="1">
         <v>0</v>
       </c>
+      <c r="FC39" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD39" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE39" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF39" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG39" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH39" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>213</v>
       </c>
@@ -20595,8 +21325,26 @@
       <c r="FB40" s="1">
         <v>0</v>
       </c>
+      <c r="FC40" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD40" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE40" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF40" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG40" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH40" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>230</v>
       </c>
@@ -21068,8 +21816,26 @@
       <c r="FB41" s="1">
         <v>0</v>
       </c>
+      <c r="FC41" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD41" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE41" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF41" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG41" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH41" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>226</v>
       </c>
@@ -21541,8 +22307,26 @@
       <c r="FB42" s="1">
         <v>0</v>
       </c>
+      <c r="FC42" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD42" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE42" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF42" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG42" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH42" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>145</v>
       </c>
@@ -22014,8 +22798,26 @@
       <c r="FB43" s="1">
         <v>0</v>
       </c>
+      <c r="FC43" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD43" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE43" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF43" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG43" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH43" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>169</v>
       </c>
@@ -22487,8 +23289,26 @@
       <c r="FB44" s="1">
         <v>0</v>
       </c>
+      <c r="FC44" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD44" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE44" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF44" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG44" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH44" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>147</v>
       </c>
@@ -22960,8 +23780,26 @@
       <c r="FB45" s="1">
         <v>0</v>
       </c>
+      <c r="FC45" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD45" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE45" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF45" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG45" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH45" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>139</v>
       </c>
@@ -23433,8 +24271,26 @@
       <c r="FB46" s="1">
         <v>0</v>
       </c>
+      <c r="FC46" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD46" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE46" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF46" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG46" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH46" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>195</v>
       </c>
@@ -23906,8 +24762,26 @@
       <c r="FB47" s="1">
         <v>0</v>
       </c>
+      <c r="FC47" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD47" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE47" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF47" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG47" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH47" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>171</v>
       </c>
@@ -24379,8 +25253,26 @@
       <c r="FB48" s="1">
         <v>0</v>
       </c>
+      <c r="FC48" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD48" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE48" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF48" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG48" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH48" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
@@ -24852,8 +25744,26 @@
       <c r="FB49" s="1">
         <v>0</v>
       </c>
+      <c r="FC49" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD49" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE49" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF49" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG49" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH49" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>161</v>
       </c>
@@ -25325,8 +26235,26 @@
       <c r="FB50" s="1">
         <v>0</v>
       </c>
+      <c r="FC50" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD50" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE50" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF50" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG50" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH50" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>236</v>
       </c>
@@ -25798,8 +26726,26 @@
       <c r="FB51" s="1">
         <v>0</v>
       </c>
+      <c r="FC51" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD51" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE51" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF51" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG51" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH51" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>193</v>
       </c>
@@ -26271,8 +27217,26 @@
       <c r="FB52" s="1">
         <v>0</v>
       </c>
+      <c r="FC52" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD52" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE52" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF52" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG52" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH52" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>250</v>
       </c>
@@ -26744,8 +27708,26 @@
       <c r="FB53" s="1">
         <v>0</v>
       </c>
+      <c r="FC53" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD53" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE53" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF53" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG53" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH53" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>149</v>
       </c>
@@ -27217,8 +28199,26 @@
       <c r="FB54" s="1">
         <v>0</v>
       </c>
+      <c r="FC54" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD54" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE54" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF54" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG54" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH54" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>137</v>
       </c>
@@ -27690,8 +28690,26 @@
       <c r="FB55" s="1">
         <v>0</v>
       </c>
+      <c r="FC55" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD55" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE55" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF55" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG55" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH55" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>181</v>
       </c>
@@ -28163,8 +29181,26 @@
       <c r="FB56" s="1">
         <v>0</v>
       </c>
+      <c r="FC56" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD56" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE56" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF56" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG56" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH56" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>232</v>
       </c>
@@ -28636,8 +29672,26 @@
       <c r="FB57" s="1">
         <v>0</v>
       </c>
+      <c r="FC57" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD57" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE57" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF57" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG57" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH57" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>234</v>
       </c>
@@ -29109,8 +30163,26 @@
       <c r="FB58" s="1">
         <v>0</v>
       </c>
+      <c r="FC58" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD58" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE58" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF58" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG58" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH58" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>215</v>
       </c>
@@ -29582,8 +30654,26 @@
       <c r="FB59" s="1">
         <v>0</v>
       </c>
+      <c r="FC59" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD59" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE59" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF59" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG59" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH59" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>185</v>
       </c>
@@ -30055,8 +31145,26 @@
       <c r="FB60" s="1">
         <v>0</v>
       </c>
+      <c r="FC60" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD60" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE60" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF60" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG60" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH60" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>246</v>
       </c>
@@ -30528,8 +31636,26 @@
       <c r="FB61" s="1">
         <v>0</v>
       </c>
+      <c r="FC61" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD61" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE61" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF61" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG61" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH61" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>191</v>
       </c>
@@ -31001,8 +32127,26 @@
       <c r="FB62" s="1">
         <v>0</v>
       </c>
+      <c r="FC62" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD62" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE62" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF62" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG62" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH62" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>248</v>
       </c>
@@ -31474,8 +32618,26 @@
       <c r="FB63" s="1">
         <v>0</v>
       </c>
+      <c r="FC63" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD63" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE63" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF63" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG63" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH63" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>252</v>
       </c>
@@ -31947,8 +33109,26 @@
       <c r="FB64" s="1">
         <v>0</v>
       </c>
+      <c r="FC64" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD64" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE64" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF64" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG64" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH64" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>173</v>
       </c>
@@ -32420,8 +33600,26 @@
       <c r="FB65" s="1">
         <v>0</v>
       </c>
+      <c r="FC65" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD65" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE65" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF65" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG65" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH65" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>254</v>
       </c>
@@ -32893,8 +34091,26 @@
       <c r="FB66" s="1">
         <v>0</v>
       </c>
+      <c r="FC66" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD66" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE66" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF66" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG66" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH66" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
@@ -33366,8 +34582,26 @@
       <c r="FB67" s="1">
         <v>0</v>
       </c>
+      <c r="FC67" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD67" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE67" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF67" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG67" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH67" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>163</v>
       </c>
@@ -33839,8 +35073,26 @@
       <c r="FB68" s="1">
         <v>0</v>
       </c>
+      <c r="FC68" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD68" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE68" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF68" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG68" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH68" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>244</v>
       </c>
@@ -34312,8 +35564,26 @@
       <c r="FB69" s="1">
         <v>0</v>
       </c>
+      <c r="FC69" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD69" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE69" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF69" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG69" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH69" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>167</v>
       </c>
@@ -34785,8 +36055,26 @@
       <c r="FB70" s="1">
         <v>0</v>
       </c>
+      <c r="FC70" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD70" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE70" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF70" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG70" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH70" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -35258,8 +36546,26 @@
       <c r="FB71" s="1">
         <v>0</v>
       </c>
+      <c r="FC71" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD71" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE71" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF71" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG71" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH71" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>165</v>
       </c>
@@ -35731,8 +37037,26 @@
       <c r="FB72" s="1">
         <v>0</v>
       </c>
+      <c r="FC72" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD72" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE72" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF72" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG72" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH72" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>187</v>
       </c>
@@ -36204,8 +37528,26 @@
       <c r="FB73" s="1">
         <v>0</v>
       </c>
+      <c r="FC73" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD73" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE73" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF73" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG73" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH73" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>219</v>
       </c>
@@ -36677,8 +38019,26 @@
       <c r="FB74" s="1">
         <v>0</v>
       </c>
+      <c r="FC74" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD74" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE74" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF74" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG74" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH74" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -37150,8 +38510,26 @@
       <c r="FB75" s="1">
         <v>0</v>
       </c>
+      <c r="FC75" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD75" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE75" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF75" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG75" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH75" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>199</v>
       </c>
@@ -37623,8 +39001,26 @@
       <c r="FB76" s="1">
         <v>0</v>
       </c>
+      <c r="FC76" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD76" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE76" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF76" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG76" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH76" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>133</v>
       </c>
@@ -38096,8 +39492,26 @@
       <c r="FB77" s="1">
         <v>0</v>
       </c>
+      <c r="FC77" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD77" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE77" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF77" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG77" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH77" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>223</v>
       </c>
@@ -38569,8 +39983,26 @@
       <c r="FB78" s="1">
         <v>0</v>
       </c>
+      <c r="FC78" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD78" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE78" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF78" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG78" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH78" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>135</v>
       </c>
@@ -39042,8 +40474,26 @@
       <c r="FB79" s="1">
         <v>0</v>
       </c>
+      <c r="FC79" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD79" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE79" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF79" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG79" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH79" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>205</v>
       </c>
@@ -39515,8 +40965,26 @@
       <c r="FB80" s="1">
         <v>0</v>
       </c>
+      <c r="FC80" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD80" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE80" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF80" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG80" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH80" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>127</v>
       </c>
@@ -39988,8 +41456,26 @@
       <c r="FB81" s="1">
         <v>0</v>
       </c>
+      <c r="FC81" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD81" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE81" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF81" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG81" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH81" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>242</v>
       </c>
@@ -40461,8 +41947,26 @@
       <c r="FB82" s="1">
         <v>0</v>
       </c>
+      <c r="FC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD82" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG82" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH82" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="83" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>155</v>
       </c>
@@ -40934,8 +42438,26 @@
       <c r="FB83" s="1">
         <v>0</v>
       </c>
+      <c r="FC83" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD83" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE83" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF83" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG83" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH83" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>143</v>
       </c>
@@ -41407,8 +42929,26 @@
       <c r="FB84" s="1">
         <v>0</v>
       </c>
+      <c r="FC84" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD84" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE84" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF84" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG84" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH84" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>256</v>
       </c>
@@ -41880,8 +43420,26 @@
       <c r="FB85" s="1">
         <v>0</v>
       </c>
+      <c r="FC85" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD85" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE85" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF85" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG85" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH85" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>28</v>
       </c>
@@ -42353,8 +43911,26 @@
       <c r="FB86" s="1">
         <v>0</v>
       </c>
+      <c r="FC86" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD86" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE86" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF86" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG86" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH86" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>77</v>
       </c>
@@ -42826,8 +44402,26 @@
       <c r="FB87" s="1">
         <v>0</v>
       </c>
+      <c r="FC87" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD87" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE87" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF87" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG87" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH87" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>197</v>
       </c>
@@ -43299,8 +44893,26 @@
       <c r="FB88" s="1">
         <v>0</v>
       </c>
+      <c r="FC88" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD88" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE88" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF88" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG88" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH88" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>228</v>
       </c>
@@ -43772,8 +45384,26 @@
       <c r="FB89" s="1">
         <v>0</v>
       </c>
+      <c r="FC89" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD89" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE89" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF89" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG89" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH89" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>175</v>
       </c>
@@ -44245,8 +45875,26 @@
       <c r="FB90" s="1">
         <v>0</v>
       </c>
+      <c r="FC90" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD90" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE90" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF90" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG90" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH90" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>179</v>
       </c>
@@ -44718,8 +46366,26 @@
       <c r="FB91" s="1">
         <v>0</v>
       </c>
+      <c r="FC91" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD91" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE91" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF91" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG91" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH91" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>201</v>
       </c>
@@ -45191,8 +46857,26 @@
       <c r="FB92" s="1">
         <v>0</v>
       </c>
+      <c r="FC92" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD92" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE92" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF92" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG92" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH92" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>238</v>
       </c>
@@ -45664,8 +47348,26 @@
       <c r="FB93" s="1">
         <v>0</v>
       </c>
+      <c r="FC93" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD93" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE93" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF93" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG93" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH93" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>183</v>
       </c>
@@ -46137,8 +47839,26 @@
       <c r="FB94" s="1">
         <v>0</v>
       </c>
+      <c r="FC94" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD94" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE94" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF94" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG94" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH94" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="95" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>203</v>
       </c>
@@ -46610,8 +48330,26 @@
       <c r="FB95" s="1">
         <v>0</v>
       </c>
+      <c r="FC95" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD95" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE95" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF95" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG95" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH95" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>141</v>
       </c>
@@ -47083,8 +48821,26 @@
       <c r="FB96" s="1">
         <v>0</v>
       </c>
+      <c r="FC96" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD96" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE96" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF96" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG96" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH96" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>240</v>
       </c>
@@ -47556,8 +49312,26 @@
       <c r="FB97" s="1">
         <v>0</v>
       </c>
+      <c r="FC97" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD97" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE97" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF97" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG97" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH97" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>209</v>
       </c>
@@ -48029,8 +49803,26 @@
       <c r="FB98" s="1">
         <v>0</v>
       </c>
+      <c r="FC98" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD98" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE98" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF98" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG98" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH98" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>32</v>
       </c>
@@ -48502,8 +50294,26 @@
       <c r="FB99" s="1">
         <v>0</v>
       </c>
+      <c r="FC99" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD99" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE99" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF99" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG99" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH99" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>41</v>
       </c>
@@ -48975,8 +50785,26 @@
       <c r="FB100" s="1">
         <v>0</v>
       </c>
+      <c r="FC100" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD100" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE100" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF100" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG100" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH100" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -49448,8 +51276,26 @@
       <c r="FB101" s="1">
         <v>0</v>
       </c>
+      <c r="FC101" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD101" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE101" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF101" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG101" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH101" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="102" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>45</v>
       </c>
@@ -49921,8 +51767,26 @@
       <c r="FB102" s="1">
         <v>0</v>
       </c>
+      <c r="FC102" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD102" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE102" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF102" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG102" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH102" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="103" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>95</v>
       </c>
@@ -50394,8 +52258,26 @@
       <c r="FB103" s="1">
         <v>0</v>
       </c>
+      <c r="FC103" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD103" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE103" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF103" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG103" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH103" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="104" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>57</v>
       </c>
@@ -50867,8 +52749,26 @@
       <c r="FB104" s="1">
         <v>0</v>
       </c>
+      <c r="FC104" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD104" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE104" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF104" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG104" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH104" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>53</v>
       </c>
@@ -51340,8 +53240,26 @@
       <c r="FB105" s="1">
         <v>0</v>
       </c>
+      <c r="FC105" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD105" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE105" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF105" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG105" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH105" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>51</v>
       </c>
@@ -51813,8 +53731,26 @@
       <c r="FB106" s="1">
         <v>0</v>
       </c>
+      <c r="FC106" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD106" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE106" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF106" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG106" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH106" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="107" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>49</v>
       </c>
@@ -52286,8 +54222,26 @@
       <c r="FB107" s="1">
         <v>0</v>
       </c>
+      <c r="FC107" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD107" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE107" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF107" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG107" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH107" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>101</v>
       </c>
@@ -52759,8 +54713,26 @@
       <c r="FB108" s="1">
         <v>0</v>
       </c>
+      <c r="FC108" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD108" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE108" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF108" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG108" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH108" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="109" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>47</v>
       </c>
@@ -53232,8 +55204,26 @@
       <c r="FB109" s="1">
         <v>0</v>
       </c>
+      <c r="FC109" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD109" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE109" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF109" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG109" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH109" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>37</v>
       </c>
@@ -53705,8 +55695,26 @@
       <c r="FB110" s="1">
         <v>0</v>
       </c>
+      <c r="FC110" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD110" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE110" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF110" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG110" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH110" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="111" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>43</v>
       </c>
@@ -54178,8 +56186,26 @@
       <c r="FB111" s="1">
         <v>0</v>
       </c>
+      <c r="FC111" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD111" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE111" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF111" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG111" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH111" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="112" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>113</v>
       </c>
@@ -54651,8 +56677,26 @@
       <c r="FB112" s="1">
         <v>0</v>
       </c>
+      <c r="FC112" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD112" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE112" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF112" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG112" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH112" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="113" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>123</v>
       </c>
@@ -55124,8 +57168,26 @@
       <c r="FB113" s="1">
         <v>0</v>
       </c>
+      <c r="FC113" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD113" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE113" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF113" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG113" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH113" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="114" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>111</v>
       </c>
@@ -55597,8 +57659,26 @@
       <c r="FB114" s="1">
         <v>0</v>
       </c>
+      <c r="FC114" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD114" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE114" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF114" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG114" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH114" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>109</v>
       </c>
@@ -56070,8 +58150,26 @@
       <c r="FB115" s="1">
         <v>0</v>
       </c>
+      <c r="FC115" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD115" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE115" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF115" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG115" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH115" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="116" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>117</v>
       </c>
@@ -56543,8 +58641,26 @@
       <c r="FB116" s="1">
         <v>0</v>
       </c>
+      <c r="FC116" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD116" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE116" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF116" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG116" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH116" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -57016,8 +59132,26 @@
       <c r="FB117" s="1">
         <v>0</v>
       </c>
+      <c r="FC117" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD117" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE117" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF117" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG117" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH117" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="118" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>93</v>
       </c>
@@ -57489,8 +59623,26 @@
       <c r="FB118" s="1">
         <v>0</v>
       </c>
+      <c r="FC118" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD118" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE118" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF118" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG118" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH118" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="119" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>119</v>
       </c>
@@ -57962,8 +60114,26 @@
       <c r="FB119" s="1">
         <v>0</v>
       </c>
+      <c r="FC119" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD119" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE119" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF119" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG119" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH119" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="120" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>107</v>
       </c>
@@ -58435,8 +60605,26 @@
       <c r="FB120" s="1">
         <v>0</v>
       </c>
+      <c r="FC120" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD120" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE120" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF120" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG120" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH120" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="121" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>97</v>
       </c>
@@ -58908,8 +61096,26 @@
       <c r="FB121" s="1">
         <v>0</v>
       </c>
+      <c r="FC121" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD121" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE121" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF121" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG121" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH121" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>115</v>
       </c>
@@ -59381,8 +61587,26 @@
       <c r="FB122" s="1">
         <v>0</v>
       </c>
+      <c r="FC122" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD122" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE122" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF122" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG122" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH122" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="123" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>105</v>
       </c>
@@ -59854,8 +62078,26 @@
       <c r="FB123" s="1">
         <v>0</v>
       </c>
+      <c r="FC123" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD123" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE123" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF123" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG123" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH123" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="124" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>125</v>
       </c>
@@ -60327,8 +62569,26 @@
       <c r="FB124" s="1">
         <v>0</v>
       </c>
+      <c r="FC124" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD124" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE124" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF124" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG124" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH124" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="125" spans="1:158" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>30</v>
       </c>
@@ -60798,6 +63058,24 @@
         <v>0</v>
       </c>
       <c r="FB125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG125" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH125" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>